<commit_message>
Changed financial projection to not have kickstarter launch
</commit_message>
<xml_diff>
--- a/presentations/financial-projections/rough-5-year-projection.xlsx
+++ b/presentations/financial-projections/rough-5-year-projection.xlsx
@@ -7,11 +7,12 @@
     <workbookView xWindow="2020" yWindow="60" windowWidth="25360" windowHeight="17240" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Revenues" sheetId="1" r:id="rId1"/>
-    <sheet name="Costs" sheetId="2" r:id="rId2"/>
+    <sheet name="Assumptions" sheetId="3" r:id="rId1"/>
+    <sheet name="Revenues" sheetId="1" r:id="rId2"/>
+    <sheet name="Costs" sheetId="2" r:id="rId3"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId3"/>
+    <externalReference r:id="rId4"/>
   </externalReferences>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -83,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="64">
   <si>
     <t>Notes</t>
   </si>
@@ -118,9 +119,6 @@
     <t>Quarterly:</t>
   </si>
   <si>
-    <t>Annual Growth Rate (after year 3):</t>
-  </si>
-  <si>
     <t>3D Scanner</t>
   </si>
   <si>
@@ -128,9 +126,6 @@
   </si>
   <si>
     <t>Price per unit</t>
-  </si>
-  <si>
-    <t>Initial Prelaunch Units:</t>
   </si>
   <si>
     <t xml:space="preserve">Total </t>
@@ -152,9 +147,6 @@
     </r>
   </si>
   <si>
-    <t>Initial quarter units (ratio of prelaunch):</t>
-  </si>
-  <si>
     <t>Annual Growth Rate Large Scan:</t>
   </si>
   <si>
@@ -264,6 +256,36 @@
   </si>
   <si>
     <t>Total Cost</t>
+  </si>
+  <si>
+    <t>Initial Annual Sales:</t>
+  </si>
+  <si>
+    <t>R&amp;D Materials</t>
+  </si>
+  <si>
+    <t>Annual growth derived from global growth of 3D printer sales from 2007 to 2011</t>
+  </si>
+  <si>
+    <t>Initial annual sales derived from current crowdfunding campaigns of competitive products</t>
+  </si>
+  <si>
+    <t>Number of employees scales to develop new products and support existing ones</t>
+  </si>
+  <si>
+    <t>Office space costs reflect the cost in Boston</t>
+  </si>
+  <si>
+    <t>Manufacturing costs lumped into unit costs</t>
+  </si>
+  <si>
+    <t>Introduce a differentiated product targeted at larger industrial customers using the same basic technology but a larger scan size</t>
+  </si>
+  <si>
+    <t>R&amp;D costs scale with revenues</t>
+  </si>
+  <si>
+    <t>1 year from beginning of summer to being able to ship a product</t>
   </si>
 </sst>
 </file>
@@ -456,7 +478,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="12">
+  <cellStyleXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
@@ -469,8 +491,10 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1"/>
@@ -526,17 +550,20 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="44" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="44" fontId="4" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="4" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="12">
+  <cellStyles count="14">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal_REVPROJ.XLS" xfId="2"/>
     <cellStyle name="Normal_SALPERS.XLS" xfId="3"/>
@@ -926,11 +953,71 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:B12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="3" spans="2:2">
+      <c r="B3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2">
+      <c r="B4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2">
+      <c r="B6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2">
+      <c r="B7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2">
+      <c r="B8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2">
+      <c r="B9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2">
+      <c r="B11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="2:2">
+      <c r="B12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1047,14 +1134,12 @@
       </c>
       <c r="M5" s="5"/>
       <c r="N5" s="5"/>
-      <c r="O5" s="11" t="s">
-        <v>11</v>
-      </c>
+      <c r="O5" s="11"/>
       <c r="P5" s="5"/>
     </row>
     <row r="6" spans="1:16">
       <c r="A6" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -1074,35 +1159,32 @@
       </c>
       <c r="M6" s="5"/>
       <c r="N6" s="5"/>
-      <c r="O6" s="5">
-        <v>1</v>
-      </c>
+      <c r="O6" s="5"/>
       <c r="P6" s="5"/>
     </row>
     <row r="7" spans="1:16">
       <c r="A7" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="13">
-        <f>$K$9*(1 + $K$12)</f>
-        <v>1500</v>
+        <v>0</v>
       </c>
       <c r="D7" s="13">
-        <f>(C37/C8)*($K$6/4 + 1)^4</f>
-        <v>4915.2000000000025</v>
+        <f>$K$9</f>
+        <v>4000</v>
       </c>
       <c r="E7" s="13">
         <f>D$7*($K$6+1)</f>
-        <v>16711.680000000008</v>
+        <v>13600</v>
       </c>
       <c r="F7" s="13">
         <f>E$7*($K$6+1)</f>
-        <v>56819.712000000021</v>
+        <v>46240</v>
       </c>
       <c r="G7" s="13">
         <f>F$7*($K$6+1)</f>
-        <v>193187.02080000006</v>
+        <v>157216</v>
       </c>
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
@@ -1116,17 +1198,15 @@
     </row>
     <row r="8" spans="1:16">
       <c r="A8" s="12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" s="3"/>
-      <c r="C8" s="14">
-        <v>500</v>
-      </c>
+      <c r="C8" s="14"/>
       <c r="D8" s="14">
         <v>500</v>
       </c>
       <c r="E8" s="14">
-        <v>450</v>
+        <v>500</v>
       </c>
       <c r="F8" s="14">
         <v>450</v>
@@ -1138,7 +1218,7 @@
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
       <c r="K8" s="11" t="s">
-        <v>15</v>
+        <v>54</v>
       </c>
       <c r="L8" s="5"/>
       <c r="M8" s="5"/>
@@ -1148,34 +1228,34 @@
     </row>
     <row r="9" spans="1:16">
       <c r="A9" s="15" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="16">
         <f>C7*C8</f>
-        <v>750000</v>
+        <v>0</v>
       </c>
       <c r="D9" s="16">
         <f>D7*D8</f>
-        <v>2457600.0000000014</v>
+        <v>2000000</v>
       </c>
       <c r="E9" s="16">
         <f>E7*E8</f>
-        <v>7520256.0000000037</v>
+        <v>6800000</v>
       </c>
       <c r="F9" s="16">
         <f>F7*F8</f>
-        <v>25568870.40000001</v>
+        <v>20808000</v>
       </c>
       <c r="G9" s="16">
         <f>G7*G8</f>
-        <v>77274808.320000023</v>
+        <v>62886400</v>
       </c>
       <c r="H9" s="17"/>
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
       <c r="K9" s="5">
-        <v>1000</v>
+        <v>4000</v>
       </c>
       <c r="L9" s="5"/>
       <c r="M9" s="5"/>
@@ -1185,7 +1265,7 @@
     </row>
     <row r="10" spans="1:16">
       <c r="A10" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="18"/>
@@ -1205,7 +1285,7 @@
     </row>
     <row r="11" spans="1:16">
       <c r="A11" s="12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="18">
@@ -1227,9 +1307,7 @@
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
-      <c r="K11" s="11" t="s">
-        <v>19</v>
-      </c>
+      <c r="K11" s="11"/>
       <c r="L11" s="5"/>
       <c r="M11" s="5"/>
       <c r="N11" s="5"/>
@@ -1238,7 +1316,7 @@
     </row>
     <row r="12" spans="1:16">
       <c r="A12" s="12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="19">
@@ -1259,9 +1337,7 @@
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
-      <c r="K12" s="5">
-        <v>0.5</v>
-      </c>
+      <c r="K12" s="5"/>
       <c r="L12" s="5"/>
       <c r="M12" s="5"/>
       <c r="N12" s="5"/>
@@ -1270,7 +1346,7 @@
     </row>
     <row r="13" spans="1:16">
       <c r="A13" s="15" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="16">
@@ -1315,10 +1391,10 @@
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
       <c r="K14" s="11" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="L14" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="M14" s="5"/>
       <c r="N14" s="5"/>
@@ -1347,28 +1423,28 @@
     </row>
     <row r="16" spans="1:16" ht="16" thickBot="1">
       <c r="A16" s="22" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="23">
         <f>C9+C13</f>
-        <v>750000</v>
+        <v>0</v>
       </c>
       <c r="D16" s="23">
         <f>D9+D13</f>
-        <v>2457600.0000000014</v>
+        <v>2000000</v>
       </c>
       <c r="E16" s="23">
         <f>E9+E13</f>
-        <v>7520256.0000000037</v>
+        <v>6800000</v>
       </c>
       <c r="F16" s="23">
         <f>F9+F13</f>
-        <v>35568870.400000006</v>
+        <v>30808000</v>
       </c>
       <c r="G16" s="23">
         <f>G9+G13</f>
-        <v>102274808.32000002</v>
+        <v>87886400</v>
       </c>
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
@@ -1421,7 +1497,7 @@
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="8" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E19" s="25"/>
       <c r="F19" s="25"/>
@@ -1458,7 +1534,7 @@
     </row>
     <row r="21" spans="1:16">
       <c r="A21" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="10" t="s">
@@ -1488,7 +1564,7 @@
     </row>
     <row r="22" spans="1:16">
       <c r="A22" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="16">
@@ -1496,7 +1572,7 @@
       </c>
       <c r="D22" s="16">
         <f>D$16*0.05</f>
-        <v>122880.00000000007</v>
+        <v>100000</v>
       </c>
       <c r="E22" s="16"/>
       <c r="F22" s="16"/>
@@ -1513,7 +1589,7 @@
     </row>
     <row r="23" spans="1:16">
       <c r="A23" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="16">
@@ -1521,7 +1597,7 @@
       </c>
       <c r="D23" s="16">
         <f>D$16*0.05</f>
-        <v>122880.00000000007</v>
+        <v>100000</v>
       </c>
       <c r="E23" s="16"/>
       <c r="F23" s="16"/>
@@ -1538,7 +1614,7 @@
     </row>
     <row r="24" spans="1:16">
       <c r="A24" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="26">
@@ -1546,7 +1622,7 @@
       </c>
       <c r="D24" s="26">
         <f>D$16*0.07</f>
-        <v>172032.00000000012</v>
+        <v>140000</v>
       </c>
       <c r="E24" s="26"/>
       <c r="F24" s="26"/>
@@ -1563,7 +1639,7 @@
     </row>
     <row r="25" spans="1:16">
       <c r="A25" s="12" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="27">
@@ -1572,19 +1648,19 @@
       </c>
       <c r="D25" s="27">
         <f>SUM(D22:D24)</f>
-        <v>417792.00000000023</v>
+        <v>340000</v>
       </c>
       <c r="E25" s="16">
         <f>E$16/(4+6*$L$6+4*$L$6^2+$L$6^3)</f>
-        <v>1121477.1919607352</v>
+        <v>1014067.1946982916</v>
       </c>
       <c r="F25" s="16">
         <f t="shared" ref="F25:G25" si="0">F$16/(4+6*$L$6+4*$L$6^2+$L$6^3)</f>
-        <v>5304297.7389875157</v>
+        <v>4594320.9020977896</v>
       </c>
       <c r="G25" s="16">
         <f t="shared" si="0"/>
-        <v>15251989.406083517</v>
+        <v>13106281.632372344</v>
       </c>
       <c r="H25" s="5"/>
       <c r="I25" s="5"/>
@@ -1598,7 +1674,7 @@
     </row>
     <row r="26" spans="1:16">
       <c r="A26" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="16">
@@ -1606,7 +1682,7 @@
       </c>
       <c r="D26" s="16">
         <f>D$16*0.06</f>
-        <v>147456.00000000009</v>
+        <v>120000</v>
       </c>
       <c r="E26" s="16"/>
       <c r="F26" s="16"/>
@@ -1623,7 +1699,7 @@
     </row>
     <row r="27" spans="1:16">
       <c r="A27" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="16">
@@ -1631,7 +1707,7 @@
       </c>
       <c r="D27" s="16">
         <f>D$16*0.07</f>
-        <v>172032.00000000012</v>
+        <v>140000</v>
       </c>
       <c r="E27" s="16"/>
       <c r="F27" s="16"/>
@@ -1648,7 +1724,7 @@
     </row>
     <row r="28" spans="1:16">
       <c r="A28" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="26">
@@ -1656,7 +1732,7 @@
       </c>
       <c r="D28" s="26">
         <f>D$16*0.07</f>
-        <v>172032.00000000012</v>
+        <v>140000</v>
       </c>
       <c r="E28" s="26"/>
       <c r="F28" s="26"/>
@@ -1673,7 +1749,7 @@
     </row>
     <row r="29" spans="1:16">
       <c r="A29" s="12" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="27">
@@ -1682,19 +1758,19 @@
       </c>
       <c r="D29" s="27">
         <f>SUM(D26:D28)</f>
-        <v>491520.00000000035</v>
+        <v>400000</v>
       </c>
       <c r="E29" s="16">
         <f>E25*(1+$L$6)</f>
-        <v>1522860.6848912316</v>
+        <v>1377007.9977676782</v>
       </c>
       <c r="F29" s="16">
         <f t="shared" ref="F29:G29" si="1">F25*(1+$L$6)</f>
-        <v>7202738.0900532417</v>
+        <v>6238656.2345921518</v>
       </c>
       <c r="G29" s="16">
         <f t="shared" si="1"/>
-        <v>20710768.974528868</v>
+        <v>17797099.366913129</v>
       </c>
       <c r="H29" s="5"/>
       <c r="I29" s="5"/>
@@ -1708,16 +1784,15 @@
     </row>
     <row r="30" spans="1:16">
       <c r="A30" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" s="16">
-        <f>$C$16*0.5</f>
-        <v>375000</v>
+        <v>0</v>
       </c>
       <c r="D30" s="16">
         <f>D$16*0.08</f>
-        <v>196608.00000000012</v>
+        <v>160000</v>
       </c>
       <c r="E30" s="16"/>
       <c r="F30" s="16"/>
@@ -1734,7 +1809,7 @@
     </row>
     <row r="31" spans="1:16">
       <c r="A31" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="16">
@@ -1742,7 +1817,7 @@
       </c>
       <c r="D31" s="16">
         <f>D$16*0.1</f>
-        <v>245760.00000000015</v>
+        <v>200000</v>
       </c>
       <c r="E31" s="16"/>
       <c r="F31" s="16"/>
@@ -1759,7 +1834,7 @@
     </row>
     <row r="32" spans="1:16">
       <c r="A32" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" s="26">
@@ -1767,7 +1842,7 @@
       </c>
       <c r="D32" s="26">
         <f>D$16*0.1</f>
-        <v>245760.00000000015</v>
+        <v>200000</v>
       </c>
       <c r="E32" s="26"/>
       <c r="F32" s="26"/>
@@ -1784,28 +1859,28 @@
     </row>
     <row r="33" spans="1:16">
       <c r="A33" s="12" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="27">
         <f>SUM(C30:C32)</f>
-        <v>375000</v>
+        <v>0</v>
       </c>
       <c r="D33" s="27">
         <f>SUM(D30:D32)</f>
-        <v>688128.00000000035</v>
+        <v>560000</v>
       </c>
       <c r="E33" s="16">
         <f>E29*(1+$L$6)</f>
-        <v>2067901.7658243973</v>
+        <v>1869847.5168406358</v>
       </c>
       <c r="F33" s="16">
         <f t="shared" ref="F33:G33" si="2">F29*(1+$L$6)</f>
-        <v>9780641.7638627067</v>
+        <v>8471509.1615921054</v>
       </c>
       <c r="G33" s="16">
         <f t="shared" si="2"/>
-        <v>28123278.878309418</v>
+        <v>24166789.235891595</v>
       </c>
       <c r="H33" s="5"/>
       <c r="I33" s="5"/>
@@ -1819,16 +1894,15 @@
     </row>
     <row r="34" spans="1:16">
       <c r="A34" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" s="16">
-        <f>C$16*0.2*$K$12</f>
-        <v>75000</v>
+        <v>0</v>
       </c>
       <c r="D34" s="16">
         <f>D$16*0.11</f>
-        <v>270336.00000000017</v>
+        <v>220000</v>
       </c>
       <c r="E34" s="16"/>
       <c r="F34" s="16"/>
@@ -1845,16 +1919,15 @@
     </row>
     <row r="35" spans="1:16">
       <c r="A35" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" s="16">
-        <f>C$16*0.3*$K$12</f>
-        <v>112500</v>
+        <v>0</v>
       </c>
       <c r="D35" s="16">
         <f>D$16*0.12</f>
-        <v>294912.00000000017</v>
+        <v>240000</v>
       </c>
       <c r="E35" s="16"/>
       <c r="F35" s="16"/>
@@ -1871,16 +1944,15 @@
     </row>
     <row r="36" spans="1:16">
       <c r="A36" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" s="16">
-        <f>C$16*0.5*$K$12</f>
-        <v>187500</v>
+        <v>0</v>
       </c>
       <c r="D36" s="26">
         <f>D$16*0.12</f>
-        <v>294912.00000000017</v>
+        <v>240000</v>
       </c>
       <c r="E36" s="26"/>
       <c r="F36" s="26"/>
@@ -1897,28 +1969,28 @@
     </row>
     <row r="37" spans="1:16">
       <c r="A37" s="12" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="27">
         <f>SUM(C34:C36)</f>
-        <v>375000</v>
+        <v>0</v>
       </c>
       <c r="D37" s="27">
         <f>SUM(D34:D36)</f>
-        <v>860160.00000000047</v>
+        <v>700000</v>
       </c>
       <c r="E37" s="16">
         <f>E33*(1+$L$6)</f>
-        <v>2808016.3573236405</v>
+        <v>2539077.2906933944</v>
       </c>
       <c r="F37" s="16">
         <f t="shared" ref="F37:G37" si="3">F33*(1+$L$6)</f>
-        <v>13281192.807096543</v>
+        <v>11503513.701717956</v>
       </c>
       <c r="G37" s="16">
         <f t="shared" si="3"/>
-        <v>38188771.061078221</v>
+        <v>32816229.76482293</v>
       </c>
       <c r="H37" s="5"/>
       <c r="I37" s="5"/>
@@ -1932,28 +2004,28 @@
     </row>
     <row r="38" spans="1:16" ht="16" thickBot="1">
       <c r="A38" s="15" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" s="28">
         <f>C25+C29+C33+C37</f>
-        <v>750000</v>
+        <v>0</v>
       </c>
       <c r="D38" s="28">
         <f>D25+D29+D33+D37</f>
-        <v>2457600.0000000014</v>
+        <v>2000000</v>
       </c>
       <c r="E38" s="28">
         <f>SUM(E25+E29+E33+E37)</f>
-        <v>7520256.0000000037</v>
+        <v>6800000</v>
       </c>
       <c r="F38" s="28">
         <f>F25+F29+F33+F37</f>
-        <v>35568870.400000006</v>
+        <v>30808000.000000007</v>
       </c>
       <c r="G38" s="28">
         <f>G25+G29+G33+G37</f>
-        <v>102274808.32000002</v>
+        <v>87886400</v>
       </c>
       <c r="H38" s="5"/>
       <c r="I38" s="5"/>
@@ -1985,7 +2057,7 @@
     </row>
     <row r="40" spans="1:16">
       <c r="A40" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" s="5"/>
@@ -2005,28 +2077,28 @@
     </row>
     <row r="41" spans="1:16">
       <c r="A41" s="12" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B41" s="29"/>
       <c r="C41" s="27">
         <f>C16/12</f>
-        <v>62500</v>
+        <v>0</v>
       </c>
       <c r="D41" s="27">
         <f>D16/12</f>
-        <v>204800.00000000012</v>
+        <v>166666.66666666666</v>
       </c>
       <c r="E41" s="27">
         <f>E16/12</f>
-        <v>626688.00000000035</v>
+        <v>566666.66666666663</v>
       </c>
       <c r="F41" s="27">
         <f>F16/12</f>
-        <v>2964072.5333333337</v>
+        <v>2567333.3333333335</v>
       </c>
       <c r="G41" s="27">
         <f>G16/12</f>
-        <v>8522900.6933333352</v>
+        <v>7323866.666666667</v>
       </c>
       <c r="H41" s="5"/>
       <c r="I41" s="5"/>
@@ -2040,28 +2112,28 @@
     </row>
     <row r="42" spans="1:16">
       <c r="A42" s="12" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B42" s="29"/>
       <c r="C42" s="27">
         <f>C16/4</f>
-        <v>187500</v>
+        <v>0</v>
       </c>
       <c r="D42" s="27">
         <f>D16/4</f>
-        <v>614400.00000000035</v>
+        <v>500000</v>
       </c>
       <c r="E42" s="27">
         <f>E16/4</f>
-        <v>1880064.0000000009</v>
+        <v>1700000</v>
       </c>
       <c r="F42" s="27">
         <f>F16/4</f>
-        <v>8892217.6000000015</v>
+        <v>7702000</v>
       </c>
       <c r="G42" s="27">
         <f>G16/4</f>
-        <v>25568702.080000006</v>
+        <v>21971600</v>
       </c>
       <c r="H42" s="2"/>
       <c r="I42" s="2"/>
@@ -2229,19 +2301,20 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="14.1640625" customWidth="1"/>
     <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.83203125" customWidth="1"/>
     <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2259,7 +2332,7 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -2311,7 +2384,7 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="12" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="32">
@@ -2332,59 +2405,59 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="13">
         <f>Revenues!C$7</f>
-        <v>1500</v>
+        <v>0</v>
       </c>
       <c r="D7" s="13">
         <f>Revenues!D$7</f>
-        <v>4915.2000000000025</v>
+        <v>4000</v>
       </c>
       <c r="E7" s="13">
         <f>Revenues!E$7</f>
-        <v>16711.680000000008</v>
+        <v>13600</v>
       </c>
       <c r="F7" s="13">
         <f>Revenues!F$7</f>
-        <v>56819.712000000021</v>
+        <v>46240</v>
       </c>
       <c r="G7" s="13">
         <f>Revenues!G$7</f>
-        <v>193187.02080000006</v>
+        <v>157216</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="30" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="18">
         <f>C$7*C$6</f>
-        <v>225000</v>
+        <v>0</v>
       </c>
       <c r="D8" s="18">
         <f t="shared" ref="D8:G8" si="0">D$7*D$6</f>
-        <v>688128.00000000035</v>
+        <v>560000</v>
       </c>
       <c r="E8" s="18">
         <f t="shared" si="0"/>
-        <v>2005401.600000001</v>
+        <v>1632000</v>
       </c>
       <c r="F8" s="18">
         <f t="shared" si="0"/>
-        <v>6250168.3200000022</v>
+        <v>5086400</v>
       </c>
       <c r="G8" s="18">
         <f t="shared" si="0"/>
-        <v>19318702.080000006</v>
+        <v>15721600</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="12" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="32">
@@ -2405,7 +2478,7 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="13">
@@ -2431,7 +2504,7 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="30" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="18">
@@ -2457,7 +2530,7 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="12" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="16">
@@ -2478,7 +2551,7 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="12" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="18">
@@ -2499,7 +2572,7 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="30" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="18">
@@ -2525,7 +2598,7 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="30" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="31">
@@ -2546,7 +2619,7 @@
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="20" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="16">
@@ -2567,7 +2640,7 @@
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="20" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="16">
@@ -2592,65 +2665,86 @@
       </c>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="15" t="s">
-        <v>56</v>
+      <c r="A18" s="20" t="s">
+        <v>55</v>
       </c>
       <c r="B18" s="3"/>
-      <c r="C18" s="21">
-        <f>C8+C11+C14+C15</f>
-        <v>475035</v>
-      </c>
-      <c r="D18" s="21">
-        <f t="shared" ref="D18:G18" si="4">D8+D11+D14+D15</f>
-        <v>1488163.0000000005</v>
-      </c>
-      <c r="E18" s="21">
+      <c r="C18" s="16">
+        <v>100000</v>
+      </c>
+      <c r="D18" s="16">
+        <v>200000</v>
+      </c>
+      <c r="E18" s="16">
+        <v>100000</v>
+      </c>
+      <c r="F18" s="16">
+        <v>2000000</v>
+      </c>
+      <c r="G18" s="16">
+        <v>5000000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" s="3"/>
+      <c r="C19" s="33">
+        <f>C8+C11+C14+C17+C18</f>
+        <v>385000</v>
+      </c>
+      <c r="D19" s="33">
+        <f t="shared" ref="D19:G19" si="4">D8+D11+D14+D17+D18</f>
+        <v>1630000</v>
+      </c>
+      <c r="E19" s="33">
         <f t="shared" si="4"/>
-        <v>3605436.600000001</v>
-      </c>
-      <c r="F18" s="21">
+        <v>3472000</v>
+      </c>
+      <c r="F19" s="33">
         <f t="shared" si="4"/>
-        <v>9850203.3200000022</v>
-      </c>
-      <c r="G18" s="21">
-        <f t="shared" si="4"/>
-        <v>25518737.080000006</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="16" thickBot="1">
-      <c r="A19" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="23">
-        <f>Revenues!C16-Costs!C18</f>
-        <v>274965</v>
-      </c>
-      <c r="D19" s="23">
-        <f>Revenues!D16-Costs!D18</f>
-        <v>969437.00000000093</v>
-      </c>
-      <c r="E19" s="23">
-        <f>Revenues!E16-Costs!E18</f>
-        <v>3914819.4000000027</v>
-      </c>
-      <c r="F19" s="23">
-        <f>Revenues!F16-Costs!F18</f>
-        <v>25718667.080000006</v>
-      </c>
-      <c r="G19" s="23">
-        <f>Revenues!G16-Costs!G18</f>
-        <v>76756071.24000001</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="16" thickTop="1">
-      <c r="A20" s="22"/>
+        <v>10896400</v>
+      </c>
+      <c r="G19" s="33">
+        <f>G8+G11+G14+G17+G18</f>
+        <v>27166600</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="16" thickBot="1">
+      <c r="A20" s="22" t="s">
+        <v>49</v>
+      </c>
       <c r="B20" s="2"/>
-      <c r="C20" s="24"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="24"/>
-      <c r="F20" s="24"/>
-      <c r="G20" s="24"/>
+      <c r="C20" s="23">
+        <f>Revenues!C16-Costs!C19</f>
+        <v>-385000</v>
+      </c>
+      <c r="D20" s="23">
+        <f>Revenues!D16-Costs!D19</f>
+        <v>370000</v>
+      </c>
+      <c r="E20" s="23">
+        <f>Revenues!E16-Costs!E19</f>
+        <v>3328000</v>
+      </c>
+      <c r="F20" s="23">
+        <f>Revenues!F16-Costs!F19</f>
+        <v>19911600</v>
+      </c>
+      <c r="G20" s="23">
+        <f>Revenues!G16-Costs!G19</f>
+        <v>60719800</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="16" thickTop="1">
+      <c r="A21" s="22"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="24"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Updated financial projections and added in weekly update
</commit_message>
<xml_diff>
--- a/presentations/financial-projections/rough-5-year-projection.xlsx
+++ b/presentations/financial-projections/rough-5-year-projection.xlsx
@@ -4,16 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2020" yWindow="60" windowWidth="25360" windowHeight="17240" tabRatio="500"/>
+    <workbookView xWindow="2020" yWindow="60" windowWidth="25360" windowHeight="17240" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Assumptions" sheetId="3" r:id="rId1"/>
     <sheet name="Revenues" sheetId="1" r:id="rId2"/>
     <sheet name="Costs" sheetId="2" r:id="rId3"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId4"/>
-  </externalReferences>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -84,10 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="64">
-  <si>
-    <t>Notes</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="65">
   <si>
     <t>Revenue Projections</t>
   </si>
@@ -129,9 +123,6 @@
   </si>
   <si>
     <t xml:space="preserve">Total </t>
-  </si>
-  <si>
-    <t>3D Scanner for Larger Objects</t>
   </si>
   <si>
     <r>
@@ -150,9 +141,6 @@
     <t>Annual Growth Rate Large Scan:</t>
   </si>
   <si>
-    <t>Quarterly</t>
-  </si>
-  <si>
     <t>Net Revenue</t>
   </si>
   <si>
@@ -279,13 +267,25 @@
     <t>Manufacturing costs lumped into unit costs</t>
   </si>
   <si>
-    <t>Introduce a differentiated product targeted at larger industrial customers using the same basic technology but a larger scan size</t>
-  </si>
-  <si>
-    <t>R&amp;D costs scale with revenues</t>
-  </si>
-  <si>
     <t>1 year from beginning of summer to being able to ship a product</t>
+  </si>
+  <si>
+    <t>Initial average salary low as we are primary initial employees, and are only paying ourselves to live</t>
+  </si>
+  <si>
+    <t>R&amp;D scale with revenues</t>
+  </si>
+  <si>
+    <t>Introduce a differentiated product targeted at larger industrial customers using the same basic technology but a larger scan size. Higher per unit margin</t>
+  </si>
+  <si>
+    <t>3D Scanner with larger scan</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> DCBA</t>
+  </si>
+  <si>
+    <t>DCBA</t>
   </si>
 </sst>
 </file>
@@ -297,7 +297,7 @@
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -356,12 +356,6 @@
       <b/>
       <sz val="10"/>
       <name val="MS Sans Serif"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
@@ -478,23 +472,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="14">
+  <cellStyleXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1"/>
@@ -532,12 +528,11 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="44" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="37" fontId="10" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="5" fontId="4" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="37" fontId="4" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="6" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
@@ -552,18 +547,20 @@
     <xf numFmtId="44" fontId="4" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="44" fontId="4" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="14">
+  <cellStyles count="16">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="14" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal_REVPROJ.XLS" xfId="2"/>
     <cellStyle name="Normal_SALPERS.XLS" xfId="3"/>
@@ -571,65 +568,6 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="WELCOME"/>
-      <sheetName val="INSTRUCTIONS"/>
-      <sheetName val="COMPS"/>
-      <sheetName val="REVENUE"/>
-      <sheetName val="COST OF REV"/>
-      <sheetName val="OPER EXP"/>
-      <sheetName val="PERSONNEL"/>
-      <sheetName val="EXTRA"/>
-      <sheetName val="TAXES"/>
-      <sheetName val="PROP &amp; EQUIP"/>
-      <sheetName val="WORKCAP"/>
-      <sheetName val="FUNDING"/>
-      <sheetName val="INCOME"/>
-      <sheetName val="BALANCE"/>
-      <sheetName val="CASHFLOW"/>
-      <sheetName val="BREAKEVEN"/>
-      <sheetName val="INCOME-MOS"/>
-      <sheetName val="CASHFLOW-MOS"/>
-      <sheetName val="SUMMARY"/>
-      <sheetName val="VAL-1"/>
-      <sheetName val="VAL-2"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2">
-        <row r="1">
-          <cell r="A1" t="str">
-            <v>DCBA</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
-      <sheetData sheetId="14" refreshError="1"/>
-      <sheetData sheetId="15" refreshError="1"/>
-      <sheetData sheetId="16" refreshError="1"/>
-      <sheetData sheetId="17" refreshError="1"/>
-      <sheetData sheetId="18" refreshError="1"/>
-      <sheetData sheetId="19" refreshError="1"/>
-      <sheetData sheetId="20" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -954,27 +892,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:B12"/>
+  <dimension ref="B3:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="3" spans="2:2">
       <c r="B3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="2:2">
       <c r="B4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="2:2">
       <c r="B6" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="2:2">
@@ -984,21 +922,26 @@
     </row>
     <row r="8" spans="2:2">
       <c r="B8" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="2:2">
       <c r="B9" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="11" spans="2:2">
-      <c r="B11" t="s">
-        <v>63</v>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2">
+      <c r="B10" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="2:2">
       <c r="B12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="2:2">
+      <c r="B13" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1017,15 +960,14 @@
   <dimension ref="A1:P50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:16" ht="21">
-      <c r="A1" s="1" t="str">
-        <f>[1]COMPS!A1</f>
-        <v>DCBA</v>
+      <c r="A1" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -1033,9 +975,7 @@
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
-      <c r="H1" s="4" t="s">
-        <v>0</v>
-      </c>
+      <c r="H1" s="4"/>
       <c r="I1" s="2"/>
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
@@ -1047,7 +987,7 @@
     </row>
     <row r="2" spans="1:16">
       <c r="A2" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -1067,7 +1007,7 @@
     </row>
     <row r="3" spans="1:16">
       <c r="A3" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="3"/>
@@ -1087,7 +1027,7 @@
     </row>
     <row r="4" spans="1:16">
       <c r="A4" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -1109,28 +1049,28 @@
       <c r="A5" s="2"/>
       <c r="B5" s="9"/>
       <c r="C5" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="E5" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="F5" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="G5" s="10" t="s">
         <v>7</v>
-      </c>
-      <c r="G5" s="10" t="s">
-        <v>8</v>
       </c>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
       <c r="K5" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="L5" s="5" t="s">
         <v>9</v>
-      </c>
-      <c r="L5" s="5" t="s">
-        <v>10</v>
       </c>
       <c r="M5" s="5"/>
       <c r="N5" s="5"/>
@@ -1139,7 +1079,7 @@
     </row>
     <row r="6" spans="1:16">
       <c r="A6" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -1164,7 +1104,7 @@
     </row>
     <row r="7" spans="1:16">
       <c r="A7" s="12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="13">
@@ -1198,10 +1138,12 @@
     </row>
     <row r="8" spans="1:16">
       <c r="A8" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" s="3"/>
-      <c r="C8" s="14"/>
+      <c r="C8" s="18">
+        <v>0</v>
+      </c>
       <c r="D8" s="14">
         <v>500</v>
       </c>
@@ -1218,7 +1160,7 @@
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
       <c r="K8" s="11" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="L8" s="5"/>
       <c r="M8" s="5"/>
@@ -1228,7 +1170,7 @@
     </row>
     <row r="9" spans="1:16">
       <c r="A9" s="15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="16">
@@ -1265,7 +1207,7 @@
     </row>
     <row r="10" spans="1:16">
       <c r="A10" s="2" t="s">
-        <v>15</v>
+        <v>62</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="18"/>
@@ -1285,7 +1227,7 @@
     </row>
     <row r="11" spans="1:16">
       <c r="A11" s="12" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="18">
@@ -1316,10 +1258,10 @@
     </row>
     <row r="12" spans="1:16">
       <c r="A12" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12" s="3"/>
-      <c r="C12" s="19">
+      <c r="C12" s="16">
         <v>0</v>
       </c>
       <c r="D12" s="16">
@@ -1346,7 +1288,7 @@
     </row>
     <row r="13" spans="1:16">
       <c r="A13" s="15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="16">
@@ -1380,7 +1322,7 @@
       <c r="P13" s="5"/>
     </row>
     <row r="14" spans="1:16">
-      <c r="A14" s="20"/>
+      <c r="A14" s="19"/>
       <c r="B14" s="3"/>
       <c r="C14" s="16"/>
       <c r="D14" s="16"/>
@@ -1391,11 +1333,9 @@
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
       <c r="K14" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="L14" s="5" t="s">
-        <v>18</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="L14" s="5"/>
       <c r="M14" s="5"/>
       <c r="N14" s="5"/>
       <c r="O14" s="5"/>
@@ -1404,11 +1344,11 @@
     <row r="15" spans="1:16">
       <c r="A15" s="15"/>
       <c r="B15" s="3"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
@@ -1422,27 +1362,27 @@
       <c r="P15" s="5"/>
     </row>
     <row r="16" spans="1:16" ht="16" thickBot="1">
-      <c r="A16" s="22" t="s">
-        <v>19</v>
+      <c r="A16" s="21" t="s">
+        <v>16</v>
       </c>
       <c r="B16" s="2"/>
-      <c r="C16" s="23">
+      <c r="C16" s="22">
         <f>C9+C13</f>
         <v>0</v>
       </c>
-      <c r="D16" s="23">
+      <c r="D16" s="22">
         <f>D9+D13</f>
         <v>2000000</v>
       </c>
-      <c r="E16" s="23">
+      <c r="E16" s="22">
         <f>E9+E13</f>
         <v>6800000</v>
       </c>
-      <c r="F16" s="23">
+      <c r="F16" s="22">
         <f>F9+F13</f>
         <v>30808000</v>
       </c>
-      <c r="G16" s="23">
+      <c r="G16" s="22">
         <f>G9+G13</f>
         <v>87886400</v>
       </c>
@@ -1457,13 +1397,13 @@
       <c r="P16" s="5"/>
     </row>
     <row r="17" spans="1:16" ht="16" thickTop="1">
-      <c r="A17" s="22"/>
+      <c r="A17" s="21"/>
       <c r="B17" s="2"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="24"/>
+      <c r="C17" s="23"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="23"/>
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
@@ -1497,10 +1437,10 @@
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
+        <v>17</v>
+      </c>
+      <c r="E19" s="24"/>
+      <c r="F19" s="24"/>
       <c r="G19" s="2"/>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
@@ -1517,10 +1457,10 @@
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="E20" s="25"/>
-      <c r="F20" s="25"/>
+        <v>2</v>
+      </c>
+      <c r="E20" s="24"/>
+      <c r="F20" s="24"/>
       <c r="G20" s="2"/>
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
@@ -1533,24 +1473,24 @@
       <c r="P20" s="5"/>
     </row>
     <row r="21" spans="1:16">
-      <c r="A21" s="22" t="s">
-        <v>21</v>
+      <c r="A21" s="21" t="s">
+        <v>18</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D21" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D21" s="10" t="s">
+      <c r="E21" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="E21" s="10" t="s">
+      <c r="F21" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F21" s="10" t="s">
+      <c r="G21" s="10" t="s">
         <v>7</v>
-      </c>
-      <c r="G21" s="10" t="s">
-        <v>8</v>
       </c>
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
@@ -1564,7 +1504,7 @@
     </row>
     <row r="22" spans="1:16">
       <c r="A22" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="16">
@@ -1589,7 +1529,7 @@
     </row>
     <row r="23" spans="1:16">
       <c r="A23" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="16">
@@ -1614,19 +1554,19 @@
     </row>
     <row r="24" spans="1:16">
       <c r="A24" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B24" s="2"/>
-      <c r="C24" s="26">
-        <v>0</v>
-      </c>
-      <c r="D24" s="26">
+      <c r="C24" s="25">
+        <v>0</v>
+      </c>
+      <c r="D24" s="25">
         <f>D$16*0.07</f>
         <v>140000</v>
       </c>
-      <c r="E24" s="26"/>
-      <c r="F24" s="26"/>
-      <c r="G24" s="26"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="25"/>
+      <c r="G24" s="25"/>
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
@@ -1639,14 +1579,14 @@
     </row>
     <row r="25" spans="1:16">
       <c r="A25" s="12" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B25" s="2"/>
-      <c r="C25" s="27">
+      <c r="C25" s="26">
         <f>SUM(C22:C24)</f>
         <v>0</v>
       </c>
-      <c r="D25" s="27">
+      <c r="D25" s="26">
         <f>SUM(D22:D24)</f>
         <v>340000</v>
       </c>
@@ -1674,7 +1614,7 @@
     </row>
     <row r="26" spans="1:16">
       <c r="A26" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="16">
@@ -1699,7 +1639,7 @@
     </row>
     <row r="27" spans="1:16">
       <c r="A27" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="16">
@@ -1724,19 +1664,19 @@
     </row>
     <row r="28" spans="1:16">
       <c r="A28" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B28" s="2"/>
-      <c r="C28" s="26">
-        <v>0</v>
-      </c>
-      <c r="D28" s="26">
+      <c r="C28" s="25">
+        <v>0</v>
+      </c>
+      <c r="D28" s="25">
         <f>D$16*0.07</f>
         <v>140000</v>
       </c>
-      <c r="E28" s="26"/>
-      <c r="F28" s="26"/>
-      <c r="G28" s="26"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="25"/>
       <c r="H28" s="5"/>
       <c r="I28" s="5"/>
       <c r="J28" s="5"/>
@@ -1749,14 +1689,14 @@
     </row>
     <row r="29" spans="1:16">
       <c r="A29" s="12" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B29" s="2"/>
-      <c r="C29" s="27">
+      <c r="C29" s="26">
         <f>SUM(C26:C28)</f>
         <v>0</v>
       </c>
-      <c r="D29" s="27">
+      <c r="D29" s="26">
         <f>SUM(D26:D28)</f>
         <v>400000</v>
       </c>
@@ -1784,7 +1724,7 @@
     </row>
     <row r="30" spans="1:16">
       <c r="A30" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" s="16">
@@ -1809,7 +1749,7 @@
     </row>
     <row r="31" spans="1:16">
       <c r="A31" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="16">
@@ -1834,19 +1774,19 @@
     </row>
     <row r="32" spans="1:16">
       <c r="A32" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B32" s="2"/>
-      <c r="C32" s="26">
-        <v>0</v>
-      </c>
-      <c r="D32" s="26">
+      <c r="C32" s="25">
+        <v>0</v>
+      </c>
+      <c r="D32" s="25">
         <f>D$16*0.1</f>
         <v>200000</v>
       </c>
-      <c r="E32" s="26"/>
-      <c r="F32" s="26"/>
-      <c r="G32" s="26"/>
+      <c r="E32" s="25"/>
+      <c r="F32" s="25"/>
+      <c r="G32" s="25"/>
       <c r="H32" s="5"/>
       <c r="I32" s="5"/>
       <c r="J32" s="5"/>
@@ -1859,14 +1799,14 @@
     </row>
     <row r="33" spans="1:16">
       <c r="A33" s="12" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B33" s="2"/>
-      <c r="C33" s="27">
+      <c r="C33" s="26">
         <f>SUM(C30:C32)</f>
         <v>0</v>
       </c>
-      <c r="D33" s="27">
+      <c r="D33" s="26">
         <f>SUM(D30:D32)</f>
         <v>560000</v>
       </c>
@@ -1894,7 +1834,7 @@
     </row>
     <row r="34" spans="1:16">
       <c r="A34" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" s="16">
@@ -1919,7 +1859,7 @@
     </row>
     <row r="35" spans="1:16">
       <c r="A35" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" s="16">
@@ -1944,19 +1884,19 @@
     </row>
     <row r="36" spans="1:16">
       <c r="A36" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" s="16">
         <v>0</v>
       </c>
-      <c r="D36" s="26">
+      <c r="D36" s="25">
         <f>D$16*0.12</f>
         <v>240000</v>
       </c>
-      <c r="E36" s="26"/>
-      <c r="F36" s="26"/>
-      <c r="G36" s="26"/>
+      <c r="E36" s="25"/>
+      <c r="F36" s="25"/>
+      <c r="G36" s="25"/>
       <c r="H36" s="5"/>
       <c r="I36" s="5"/>
       <c r="J36" s="5"/>
@@ -1969,14 +1909,14 @@
     </row>
     <row r="37" spans="1:16">
       <c r="A37" s="12" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B37" s="2"/>
-      <c r="C37" s="27">
+      <c r="C37" s="26">
         <f>SUM(C34:C36)</f>
         <v>0</v>
       </c>
-      <c r="D37" s="27">
+      <c r="D37" s="26">
         <f>SUM(D34:D36)</f>
         <v>700000</v>
       </c>
@@ -2004,26 +1944,26 @@
     </row>
     <row r="38" spans="1:16" ht="16" thickBot="1">
       <c r="A38" s="15" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B38" s="2"/>
-      <c r="C38" s="28">
+      <c r="C38" s="27">
         <f>C25+C29+C33+C37</f>
         <v>0</v>
       </c>
-      <c r="D38" s="28">
+      <c r="D38" s="27">
         <f>D25+D29+D33+D37</f>
         <v>2000000</v>
       </c>
-      <c r="E38" s="28">
+      <c r="E38" s="27">
         <f>SUM(E25+E29+E33+E37)</f>
         <v>6800000</v>
       </c>
-      <c r="F38" s="28">
+      <c r="F38" s="27">
         <f>F25+F29+F33+F37</f>
         <v>30808000.000000007</v>
       </c>
-      <c r="G38" s="28">
+      <c r="G38" s="27">
         <f>G25+G29+G33+G37</f>
         <v>87886400</v>
       </c>
@@ -2057,7 +1997,7 @@
     </row>
     <row r="40" spans="1:16">
       <c r="A40" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" s="5"/>
@@ -2077,26 +2017,26 @@
     </row>
     <row r="41" spans="1:16">
       <c r="A41" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="B41" s="29"/>
-      <c r="C41" s="27">
+        <v>37</v>
+      </c>
+      <c r="B41" s="28"/>
+      <c r="C41" s="26">
         <f>C16/12</f>
         <v>0</v>
       </c>
-      <c r="D41" s="27">
+      <c r="D41" s="26">
         <f>D16/12</f>
         <v>166666.66666666666</v>
       </c>
-      <c r="E41" s="27">
+      <c r="E41" s="26">
         <f>E16/12</f>
         <v>566666.66666666663</v>
       </c>
-      <c r="F41" s="27">
+      <c r="F41" s="26">
         <f>F16/12</f>
         <v>2567333.3333333335</v>
       </c>
-      <c r="G41" s="27">
+      <c r="G41" s="26">
         <f>G16/12</f>
         <v>7323866.666666667</v>
       </c>
@@ -2112,26 +2052,26 @@
     </row>
     <row r="42" spans="1:16">
       <c r="A42" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="B42" s="29"/>
-      <c r="C42" s="27">
+        <v>38</v>
+      </c>
+      <c r="B42" s="28"/>
+      <c r="C42" s="26">
         <f>C16/4</f>
         <v>0</v>
       </c>
-      <c r="D42" s="27">
+      <c r="D42" s="26">
         <f>D16/4</f>
         <v>500000</v>
       </c>
-      <c r="E42" s="27">
+      <c r="E42" s="26">
         <f>E16/4</f>
         <v>1700000</v>
       </c>
-      <c r="F42" s="27">
+      <c r="F42" s="26">
         <f>F16/4</f>
         <v>7702000</v>
       </c>
-      <c r="G42" s="27">
+      <c r="G42" s="26">
         <f>G16/4</f>
         <v>21971600</v>
       </c>
@@ -2305,8 +2245,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2319,9 +2259,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21">
-      <c r="A1" s="1" t="str">
-        <f>[1]COMPS!A1</f>
-        <v>DCBA</v>
+      <c r="A1" s="1" t="s">
+        <v>64</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -2332,7 +2271,7 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -2343,7 +2282,7 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="3"/>
@@ -2354,7 +2293,7 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -2367,45 +2306,45 @@
       <c r="A5" s="2"/>
       <c r="B5" s="9"/>
       <c r="C5" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="E5" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="F5" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="G5" s="10" t="s">
         <v>7</v>
-      </c>
-      <c r="G5" s="10" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="12" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B6" s="2"/>
-      <c r="C6" s="32">
+      <c r="C6" s="31">
         <v>150</v>
       </c>
-      <c r="D6" s="32">
+      <c r="D6" s="31">
         <v>140</v>
       </c>
-      <c r="E6" s="32">
+      <c r="E6" s="31">
         <v>120</v>
       </c>
-      <c r="F6" s="32">
+      <c r="F6" s="31">
         <v>110</v>
       </c>
-      <c r="G6" s="32">
+      <c r="G6" s="31">
         <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="13">
@@ -2430,8 +2369,8 @@
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="30" t="s">
-        <v>43</v>
+      <c r="A8" s="29" t="s">
+        <v>40</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="18">
@@ -2457,28 +2396,28 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="12" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B9" s="2"/>
-      <c r="C9" s="32">
-        <v>0</v>
-      </c>
-      <c r="D9" s="32">
-        <v>0</v>
-      </c>
-      <c r="E9" s="32">
-        <v>0</v>
-      </c>
-      <c r="F9" s="32">
+      <c r="C9" s="31">
+        <v>0</v>
+      </c>
+      <c r="D9" s="31">
+        <v>0</v>
+      </c>
+      <c r="E9" s="31">
+        <v>0</v>
+      </c>
+      <c r="F9" s="31">
         <v>300</v>
       </c>
-      <c r="G9" s="32">
+      <c r="G9" s="31">
         <v>300</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="13">
@@ -2503,8 +2442,8 @@
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="30" t="s">
-        <v>43</v>
+      <c r="A11" s="29" t="s">
+        <v>40</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="18">
@@ -2530,7 +2469,7 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="12" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="16">
@@ -2551,28 +2490,28 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="12" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="18">
         <v>50000</v>
       </c>
       <c r="D13" s="18">
-        <v>80000</v>
+        <v>100000</v>
       </c>
       <c r="E13" s="18">
-        <v>80000</v>
+        <v>120000</v>
       </c>
       <c r="F13" s="18">
-        <v>70000</v>
+        <v>150000</v>
       </c>
       <c r="G13" s="18">
-        <v>70000</v>
+        <v>150000</v>
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="30" t="s">
-        <v>48</v>
+      <c r="A14" s="29" t="s">
+        <v>45</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="18">
@@ -2581,45 +2520,45 @@
       </c>
       <c r="D14" s="18">
         <f t="shared" ref="D14:G14" si="2">D13*D12</f>
-        <v>800000</v>
+        <v>1000000</v>
       </c>
       <c r="E14" s="18">
         <f t="shared" si="2"/>
-        <v>1600000</v>
+        <v>2400000</v>
       </c>
       <c r="F14" s="18">
         <f t="shared" si="2"/>
-        <v>2100000</v>
+        <v>4500000</v>
       </c>
       <c r="G14" s="18">
         <f t="shared" si="2"/>
-        <v>2450000</v>
+        <v>5250000</v>
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="30" t="s">
-        <v>50</v>
+      <c r="A15" s="29" t="s">
+        <v>47</v>
       </c>
       <c r="B15" s="3"/>
-      <c r="C15" s="31">
+      <c r="C15" s="30">
         <v>35</v>
       </c>
-      <c r="D15" s="31">
+      <c r="D15" s="30">
         <v>35</v>
       </c>
-      <c r="E15" s="31">
+      <c r="E15" s="30">
         <v>35</v>
       </c>
-      <c r="F15" s="31">
+      <c r="F15" s="30">
         <v>35</v>
       </c>
-      <c r="G15" s="31">
+      <c r="G15" s="30">
         <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="20" t="s">
-        <v>51</v>
+      <c r="A16" s="19" t="s">
+        <v>48</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="16">
@@ -2639,8 +2578,8 @@
       </c>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="20" t="s">
-        <v>52</v>
+      <c r="A17" s="19" t="s">
+        <v>49</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="16">
@@ -2665,8 +2604,8 @@
       </c>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="20" t="s">
-        <v>55</v>
+      <c r="A18" s="19" t="s">
+        <v>52</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="16">
@@ -2687,64 +2626,64 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="15" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B19" s="3"/>
-      <c r="C19" s="33">
+      <c r="C19" s="32">
         <f>C8+C11+C14+C17+C18</f>
         <v>385000</v>
       </c>
-      <c r="D19" s="33">
-        <f t="shared" ref="D19:G19" si="4">D8+D11+D14+D17+D18</f>
-        <v>1630000</v>
-      </c>
-      <c r="E19" s="33">
+      <c r="D19" s="32">
+        <f t="shared" ref="D19:F19" si="4">D8+D11+D14+D17+D18</f>
+        <v>1830000</v>
+      </c>
+      <c r="E19" s="32">
         <f t="shared" si="4"/>
-        <v>3472000</v>
-      </c>
-      <c r="F19" s="33">
+        <v>4272000</v>
+      </c>
+      <c r="F19" s="32">
         <f t="shared" si="4"/>
-        <v>10896400</v>
-      </c>
-      <c r="G19" s="33">
+        <v>13296400</v>
+      </c>
+      <c r="G19" s="32">
         <f>G8+G11+G14+G17+G18</f>
-        <v>27166600</v>
+        <v>29966600</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="16" thickBot="1">
-      <c r="A20" s="22" t="s">
-        <v>49</v>
+      <c r="A20" s="21" t="s">
+        <v>46</v>
       </c>
       <c r="B20" s="2"/>
-      <c r="C20" s="23">
+      <c r="C20" s="22">
         <f>Revenues!C16-Costs!C19</f>
         <v>-385000</v>
       </c>
-      <c r="D20" s="23">
+      <c r="D20" s="22">
         <f>Revenues!D16-Costs!D19</f>
-        <v>370000</v>
-      </c>
-      <c r="E20" s="23">
+        <v>170000</v>
+      </c>
+      <c r="E20" s="22">
         <f>Revenues!E16-Costs!E19</f>
-        <v>3328000</v>
-      </c>
-      <c r="F20" s="23">
+        <v>2528000</v>
+      </c>
+      <c r="F20" s="22">
         <f>Revenues!F16-Costs!F19</f>
-        <v>19911600</v>
-      </c>
-      <c r="G20" s="23">
+        <v>17511600</v>
+      </c>
+      <c r="G20" s="22">
         <f>Revenues!G16-Costs!G19</f>
-        <v>60719800</v>
+        <v>57919800</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="16" thickTop="1">
-      <c r="A21" s="22"/>
+      <c r="A21" s="21"/>
       <c r="B21" s="2"/>
-      <c r="C21" s="24"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="24"/>
-      <c r="F21" s="24"/>
-      <c r="G21" s="24"/>
+      <c r="C21" s="23"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="23"/>
+      <c r="G21" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>